<commit_message>
#60 Excel data source
</commit_message>
<xml_diff>
--- a/runner/src/test/resources/test_projects/Fifa2019/fifaranking2019.xlsx
+++ b/runner/src/test/resources/test_projects/Fifa2019/fifaranking2019.xlsx
@@ -194,10 +194,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -216,36 +216,21 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="n">
-        <v>1746</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -254,16 +239,10 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>2</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="3" t="n">
-        <v>1718</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -272,16 +251,10 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="3" t="n">
-        <v>1681</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -290,137 +263,217 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>345</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>1746</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="n">
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>340</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>1718</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>240</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>1681</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>123</v>
+      </c>
+      <c r="H10" s="3" t="n">
         <v>1652</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="n">
+      <c r="G11" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="H11" s="3" t="n">
         <v>1631</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="n">
+      <c r="G12" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H12" s="3" t="n">
         <v>1625</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="F13" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="n">
+      <c r="G13" s="4" t="n">
+        <v>56</v>
+      </c>
+      <c r="H13" s="3" t="n">
         <v>1617</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="n">
+      <c r="G14" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="H14" s="3" t="n">
         <v>1615</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="n">
+      <c r="G15" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="H15" s="3" t="n">
         <v>1605</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3" t="n">
+      <c r="G16" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="H16" s="3" t="n">
         <v>1589</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="Belgium"/>
-    <hyperlink ref="D4" r:id="rId2" display="France"/>
-    <hyperlink ref="D5" r:id="rId3" display="Brazil"/>
-    <hyperlink ref="D6" r:id="rId4" display="England"/>
-    <hyperlink ref="D7" r:id="rId5" display="Portugal"/>
-    <hyperlink ref="D8" r:id="rId6" display="Croatia"/>
-    <hyperlink ref="D9" r:id="rId7" display="Spain"/>
-    <hyperlink ref="D10" r:id="rId8" display="Uruguay"/>
-    <hyperlink ref="D11" r:id="rId9" display="Switzerland"/>
-    <hyperlink ref="D12" r:id="rId10" display="Denmark"/>
+    <hyperlink ref="I7" r:id="rId1" display="Belgium"/>
+    <hyperlink ref="I8" r:id="rId2" display="France"/>
+    <hyperlink ref="I9" r:id="rId3" display="Brazil"/>
+    <hyperlink ref="I10" r:id="rId4" display="England"/>
+    <hyperlink ref="I11" r:id="rId5" display="Portugal"/>
+    <hyperlink ref="I12" r:id="rId6" display="Croatia"/>
+    <hyperlink ref="I13" r:id="rId7" display="Spain"/>
+    <hyperlink ref="I14" r:id="rId8" display="Uruguay"/>
+    <hyperlink ref="I15" r:id="rId9" display="Switzerland"/>
+    <hyperlink ref="I16" r:id="rId10" display="Denmark"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
#60 Adding test coverage
</commit_message>
<xml_diff>
--- a/runner/src/test/resources/test_projects/Fifa2019/fifaranking2019.xlsx
+++ b/runner/src/test/resources/test_projects/Fifa2019/fifaranking2019.xlsx
@@ -197,12 +197,12 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
#61 Java format + test Excel cell formula
</commit_message>
<xml_diff>
--- a/runner/src/test/resources/test_projects/Fifa2019/fifaranking2019.xlsx
+++ b/runner/src/test/resources/test_projects/Fifa2019/fifaranking2019.xlsx
@@ -197,7 +197,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -312,7 +312,8 @@
         <v>2</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>340</v>
+        <f aca="false">G7- 15</f>
+        <v>330</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>1718</v>
@@ -352,7 +353,8 @@
         <v>4</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>123</v>
+        <f aca="false">G9- 15</f>
+        <v>225</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>1652</v>
@@ -411,7 +413,8 @@
         <v>7</v>
       </c>
       <c r="G13" s="4" t="n">
-        <v>56</v>
+        <f aca="false">G12- 15</f>
+        <v>85</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>1617</v>

</xml_diff>